<commit_message>
1. Added model for biomass and used values as per Marieke's calculation
</commit_message>
<xml_diff>
--- a/biomass/Biomass.xlsx
+++ b/biomass/Biomass.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Biofuels" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Biofuels" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="100">
   <si>
     <t>Region</t>
   </si>
@@ -324,12 +325,21 @@
   <si>
     <t>Total Demand</t>
   </si>
+  <si>
+    <t>Planting time</t>
+  </si>
+  <si>
+    <t>Harvesting time</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,6 +372,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,13 +555,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -583,15 +604,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -600,9 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -613,10 +622,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -932,7 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI62"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
@@ -10182,8 +10215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW7"/>
   <sheetViews>
-    <sheetView topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD25" sqref="AD25"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AR3" sqref="AR3:AU7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10202,68 +10235,68 @@
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="45"/>
       <c r="D1" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33" t="s">
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33" t="s">
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33" t="s">
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33" t="s">
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="37"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="34"/>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A2" s="32"/>
@@ -10402,10 +10435,10 @@
       <c r="AT2" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="AU2" s="36" t="s">
+      <c r="AU2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="AV2" s="37"/>
+      <c r="AV2" s="34"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -11079,105 +11112,689 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AM1:AU1"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="U1:AC1"/>
     <mergeCell ref="AD1:AL1"/>
-    <mergeCell ref="AM1:AU1"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="43">
+        <v>1</v>
+      </c>
+      <c r="C2" s="43">
+        <v>3150</v>
+      </c>
+      <c r="D2" s="43">
+        <v>7278</v>
+      </c>
+      <c r="E2" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F2" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G2" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43">
+        <v>2</v>
+      </c>
+      <c r="C3" s="43">
+        <v>3172</v>
+      </c>
+      <c r="D3" s="43">
+        <v>7104</v>
+      </c>
+      <c r="E3" s="43">
+        <v>2.5000000000000005E-2</v>
+      </c>
+      <c r="F3" s="43">
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="G3" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43">
+        <v>3</v>
+      </c>
+      <c r="C4" s="43">
+        <v>2880</v>
+      </c>
+      <c r="D4" s="43">
+        <v>6728</v>
+      </c>
+      <c r="E4" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F4" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G4" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43">
+        <v>4</v>
+      </c>
+      <c r="C5" s="43">
+        <v>2472</v>
+      </c>
+      <c r="D5" s="43">
+        <v>6069</v>
+      </c>
+      <c r="E5" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F5" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G5" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43">
+        <v>5</v>
+      </c>
+      <c r="C6" s="43">
+        <v>2592</v>
+      </c>
+      <c r="D6" s="43">
+        <v>6584</v>
+      </c>
+      <c r="E6" s="43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F6" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="43">
+        <v>1</v>
+      </c>
+      <c r="C7" s="43">
+        <v>1284</v>
+      </c>
+      <c r="D7" s="43">
+        <v>2538</v>
+      </c>
+      <c r="E7" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F7" s="43">
+        <v>0.17998560115190784</v>
+      </c>
+      <c r="G7" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43">
+        <v>2</v>
+      </c>
+      <c r="C8" s="43">
+        <v>3220</v>
+      </c>
+      <c r="D8" s="43">
+        <v>6430</v>
+      </c>
+      <c r="E8" s="43">
+        <v>2.5000000000000005E-2</v>
+      </c>
+      <c r="F8" s="43">
+        <v>0.17998560115190776</v>
+      </c>
+      <c r="G8" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43">
+        <v>3</v>
+      </c>
+      <c r="C9" s="43">
+        <v>3216</v>
+      </c>
+      <c r="D9" s="43">
+        <v>6736</v>
+      </c>
+      <c r="E9" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F9" s="43">
+        <v>0.17998560115190784</v>
+      </c>
+      <c r="G9" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43">
+        <v>4</v>
+      </c>
+      <c r="C10" s="43">
+        <v>3604</v>
+      </c>
+      <c r="D10" s="43">
+        <v>7267</v>
+      </c>
+      <c r="E10" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F10" s="43">
+        <v>0.17998560115190784</v>
+      </c>
+      <c r="G10" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="43"/>
+      <c r="B11" s="43">
+        <v>5</v>
+      </c>
+      <c r="C11" s="43">
+        <v>2856</v>
+      </c>
+      <c r="D11" s="43">
+        <v>6264</v>
+      </c>
+      <c r="E11" s="43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F11" s="43">
+        <v>0.17998560115190784</v>
+      </c>
+      <c r="G11" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="43">
+        <v>1</v>
+      </c>
+      <c r="C12" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D12" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E12" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F12" s="43">
+        <v>0.30400000000000005</v>
+      </c>
+      <c r="G12" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43">
+        <v>2</v>
+      </c>
+      <c r="C13" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D13" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E13" s="43">
+        <v>2.5000000000000005E-2</v>
+      </c>
+      <c r="F13" s="43">
+        <v>0.30400000000000016</v>
+      </c>
+      <c r="G13" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43">
+        <v>3</v>
+      </c>
+      <c r="C14" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D14" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E14" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F14" s="43">
+        <v>0.30400000000000005</v>
+      </c>
+      <c r="G14" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43">
+        <v>4</v>
+      </c>
+      <c r="C15" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D15" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E15" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F15" s="43">
+        <v>0.3040000000000001</v>
+      </c>
+      <c r="G15" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="43"/>
+      <c r="B16" s="43">
+        <v>5</v>
+      </c>
+      <c r="C16" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D16" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E16" s="43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F16" s="43">
+        <v>0.30400000000000005</v>
+      </c>
+      <c r="G16" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="43">
+        <v>1</v>
+      </c>
+      <c r="C17" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D17" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E17" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F17" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G17" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43">
+        <v>2</v>
+      </c>
+      <c r="C18" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D18" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E18" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F18" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G18" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="43"/>
+      <c r="B19" s="43">
+        <v>3</v>
+      </c>
+      <c r="C19" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D19" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E19" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F19" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G19" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43">
+        <v>4</v>
+      </c>
+      <c r="C20" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D20" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E20" s="43">
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="F20" s="43">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="G20" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43">
+        <v>5</v>
+      </c>
+      <c r="C21" s="43">
+        <v>2976</v>
+      </c>
+      <c r="D21" s="43">
+        <v>5304</v>
+      </c>
+      <c r="E21" s="43">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F21" s="43">
+        <v>0.4</v>
+      </c>
+      <c r="G21" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="43">
+        <v>1</v>
+      </c>
+      <c r="C22" s="43">
+        <v>0</v>
+      </c>
+      <c r="D22" s="43">
+        <v>0</v>
+      </c>
+      <c r="E22" s="43">
+        <v>0</v>
+      </c>
+      <c r="F22" s="43">
+        <v>0</v>
+      </c>
+      <c r="G22" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43">
+        <v>2</v>
+      </c>
+      <c r="C23" s="43">
+        <v>0</v>
+      </c>
+      <c r="D23" s="43">
+        <v>0</v>
+      </c>
+      <c r="E23" s="43">
+        <v>0</v>
+      </c>
+      <c r="F23" s="43">
+        <v>0</v>
+      </c>
+      <c r="G23" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="43"/>
+      <c r="B24" s="43">
+        <v>3</v>
+      </c>
+      <c r="C24" s="43">
+        <v>0</v>
+      </c>
+      <c r="D24" s="43">
+        <v>0</v>
+      </c>
+      <c r="E24" s="43">
+        <v>0</v>
+      </c>
+      <c r="F24" s="43">
+        <v>0</v>
+      </c>
+      <c r="G24" s="43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="43"/>
+      <c r="B25" s="43">
+        <v>4</v>
+      </c>
+      <c r="C25" s="43">
+        <v>1</v>
+      </c>
+      <c r="D25" s="43">
+        <v>8760</v>
+      </c>
+      <c r="E25" s="43">
+        <v>0.01</v>
+      </c>
+      <c r="F25" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="43"/>
+      <c r="B26" s="43">
+        <v>5</v>
+      </c>
+      <c r="C26" s="43">
+        <v>1</v>
+      </c>
+      <c r="D26" s="43">
+        <v>8760</v>
+      </c>
+      <c r="E26" s="43">
+        <v>0.01</v>
+      </c>
+      <c r="F26" s="43">
+        <v>0.3</v>
+      </c>
+      <c r="G26" s="43">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="40" customWidth="1"/>
-    <col min="2" max="4" width="10.83203125" style="40"/>
-    <col min="5" max="5" width="8.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="40"/>
-    <col min="7" max="7" width="8.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="40"/>
-    <col min="9" max="9" width="8.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="40"/>
-    <col min="11" max="11" width="8.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="40"/>
+    <col min="1" max="1" width="11.5" style="37" customWidth="1"/>
+    <col min="2" max="4" width="10.83203125" style="37"/>
+    <col min="5" max="5" width="8.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="37"/>
+    <col min="7" max="7" width="8.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="37"/>
+    <col min="9" max="9" width="8.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="37"/>
+    <col min="11" max="11" width="8.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="39"/>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="36"/>
+      <c r="B1" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41" t="s">
+      <c r="E1" s="47"/>
+      <c r="F1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41" t="s">
+      <c r="I1" s="47"/>
+      <c r="J1" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="41"/>
+      <c r="K1" s="47"/>
     </row>
     <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="43" t="s">
+      <c r="K2" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="36">
         <v>0.23121489609766199</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="36">
         <v>8098576.2320000008</v>
       </c>
       <c r="D3">
@@ -11206,13 +11823,13 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="40">
         <v>4.9636436929999999</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="40">
         <v>2067438</v>
       </c>
       <c r="D4">
@@ -11241,13 +11858,13 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="36">
         <v>23.5653015269333</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="36">
         <v>4224</v>
       </c>
       <c r="D5">
@@ -11276,25 +11893,25 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="39">
-        <v>0</v>
-      </c>
-      <c r="C6" s="39">
+      <c r="B6" s="36">
+        <v>0</v>
+      </c>
+      <c r="C6" s="36">
         <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="36">
         <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="36">
         <v>0</v>
       </c>
       <c r="H6">
@@ -11311,80 +11928,80 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="36">
         <f>SUM(B3:B6)</f>
         <v>28.760160116030963</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="36">
         <f t="shared" ref="C8:K8" si="0">SUM(C3:C6)</f>
         <v>10170238.232000001</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="36">
         <f t="shared" si="0"/>
         <v>24.780055859696422</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="36">
         <f t="shared" si="0"/>
         <v>22545209.655500006</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="36">
         <f t="shared" si="0"/>
         <v>40.868919031974393</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="36">
         <f t="shared" si="0"/>
         <v>3795991.7634999999</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="36">
         <f t="shared" si="0"/>
         <v>31.787662216739314</v>
       </c>
-      <c r="I8" s="39">
+      <c r="I8" s="36">
         <f t="shared" si="0"/>
         <v>73670747.569499999</v>
       </c>
-      <c r="J8" s="39">
+      <c r="J8" s="36">
         <f t="shared" si="0"/>
         <v>32.680293842111574</v>
       </c>
-      <c r="K8" s="39">
+      <c r="K8" s="36">
         <f t="shared" si="0"/>
         <v>233206.16091648102</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="37">
         <v>39.1</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="37">
         <v>274</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="37">
         <v>202</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="37">
         <v>168</v>
       </c>
-      <c r="J9" s="40">
+      <c r="J9" s="37">
         <v>110</v>
       </c>
     </row>

</xml_diff>